<commit_message>
修正 convert.js 使其能轉換多個 imagesUrls
</commit_message>
<xml_diff>
--- a/w2/products.xlsx
+++ b/w2/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyeh\Desktop\React_hw\w2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2DEBB-2857-4322-B10B-1914D82F5123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8677CD15-E96C-41D4-8351-7C97B1591439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,6 @@
     <t>imageUrl</t>
   </si>
   <si>
-    <t>imageUrls</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>抹茶</t>
   </si>
   <si>
@@ -270,6 +266,10 @@
   </si>
   <si>
     <t>https://images.unsplash.com/photo-1563791136187-40150b71f6f5?q=80&amp;w=300&amp;auto=format&amp;fit=crop&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D,https://images.unsplash.com/photo-1579349443343-73da56a71a20?q=80&amp;w=400&amp;auto=format&amp;fit=crop&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxwaG90by1wYWdlfHx8fGVufDB8fHx8fA%3D%3D</t>
+  </si>
+  <si>
+    <t>imagesUrls</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -698,27 +698,27 @@
         <v>8</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>150</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -727,30 +727,30 @@
         <v>100</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="E3" s="1">
         <v>200</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3">
         <v>100</v>
@@ -759,30 +759,30 @@
         <v>55</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="E4" s="1">
         <v>55</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="3">
         <v>300</v>
@@ -791,30 +791,30 @@
         <v>150</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="E5" s="1">
         <v>20</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="3">
         <v>150</v>
@@ -823,30 +823,30 @@
         <v>120</v>
       </c>
       <c r="I5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1">
         <v>100</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="3">
         <v>60</v>
@@ -855,30 +855,30 @@
         <v>30</v>
       </c>
       <c r="I6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1">
         <v>66</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3">
         <v>55</v>
@@ -887,30 +887,30 @@
         <v>35</v>
       </c>
       <c r="I7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="E8" s="1">
         <v>37</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3">
         <v>150</v>
@@ -919,30 +919,30 @@
         <v>85</v>
       </c>
       <c r="I8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1">
         <v>65</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="3">
         <v>180</v>
@@ -951,30 +951,30 @@
         <v>100</v>
       </c>
       <c r="I9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="D10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1">
         <v>92</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="3">
         <v>500</v>
@@ -983,30 +983,30 @@
         <v>350</v>
       </c>
       <c r="I10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1">
         <v>55</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" s="3">
         <v>250</v>
@@ -1015,10 +1015,10 @@
         <v>150</v>
       </c>
       <c r="I11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">

</xml_diff>